<commit_message>
feat(option): 新增类型 数组  基础类型[]    字典 dic<int32, int32>  map<int32, int32>  <int32, int32>
</commit_message>
<xml_diff>
--- a/Assets/Excel/ExampleData22.xlsx
+++ b/Assets/Excel/ExampleData22.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E666BBE0-57D4-6845-9D0E-20E11693EC72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D4A493-5A5C-2944-9F90-18522F55AC1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="2400" windowWidth="27120" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,6 +234,62 @@
   </si>
   <si>
     <t>c#Enemy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinalTest1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12|13|14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31|33|34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinalTest2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;string, string&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinalTest3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dic&lt;string, string&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FinalTest4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32[]类型测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;string, string&gt;类型测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dic&lt;string, string&gt;类型测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32类型测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -666,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -685,7 +741,7 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -725,8 +781,20 @@
       <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -766,8 +834,20 @@
       <c r="M2" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -807,8 +887,20 @@
       <c r="M3" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -848,8 +940,20 @@
       <c r="M4" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -889,8 +993,20 @@
       <c r="M5" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>66</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:17">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -927,6 +1043,18 @@
       </c>
       <c r="M6" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>